<commit_message>
some changes and corrections
</commit_message>
<xml_diff>
--- a/hardware/Datasheet/berechnungen.xlsx
+++ b/hardware/Datasheet/berechnungen.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A951BC2A-09E6-4C80-BAA3-332C9FFE93BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D45516-964E-4F41-83A0-11D27DB1E505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PWM" sheetId="1" r:id="rId1"/>
-    <sheet name="ADC" sheetId="2" r:id="rId2"/>
-    <sheet name="Lambda DAC" sheetId="5" r:id="rId3"/>
-    <sheet name="LSU 4.9 Pinout" sheetId="3" r:id="rId4"/>
-    <sheet name="HEX" sheetId="4" r:id="rId5"/>
+    <sheet name="Ip" sheetId="6" r:id="rId2"/>
+    <sheet name="ADC" sheetId="2" r:id="rId3"/>
+    <sheet name="Lambda DAC" sheetId="5" r:id="rId4"/>
+    <sheet name="LSU 4.9 Pinout" sheetId="3" r:id="rId5"/>
+    <sheet name="HEX" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
   <si>
     <t>Fcpu</t>
   </si>
@@ -248,6 +249,39 @@
   </si>
   <si>
     <t>Drift, mV</t>
+  </si>
+  <si>
+    <t>Spannung Referenz, mV</t>
+  </si>
+  <si>
+    <t>ADC Wert dazu:</t>
+  </si>
+  <si>
+    <t>Spannung Referenz gemessen</t>
+  </si>
+  <si>
+    <t>Drift:</t>
+  </si>
+  <si>
+    <t>Shunt</t>
+  </si>
+  <si>
+    <t>Ua</t>
+  </si>
+  <si>
+    <t>Ua_ref</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>divisor</t>
+  </si>
+  <si>
+    <t>Amp</t>
+  </si>
+  <si>
+    <t>Ip</t>
   </si>
 </sst>
 </file>
@@ -742,16 +776,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED533D4-38E1-42C6-9DE3-B349AD92F31E}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1">
+        <v>61900</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3">
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5">
+        <f>(B3-B4)*1000</f>
+        <v>566000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6">
+        <f>B1*B2</f>
+        <v>495200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7">
+        <f>B5/B6*1000</f>
+        <v>1142.9725363489499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -851,7 +960,7 @@
         <v>40</v>
       </c>
       <c r="B15">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -860,7 +969,7 @@
       </c>
       <c r="B16">
         <f>(5/1024)*B15</f>
-        <v>1.201171875</v>
+        <v>1.2060546875</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -869,7 +978,7 @@
       </c>
       <c r="B17">
         <f>B16 - 1.225</f>
-        <v>-2.3828125000000089E-2</v>
+        <v>-1.8945312500000089E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -902,7 +1011,7 @@
       </c>
       <c r="B22">
         <f>C19-B17</f>
-        <v>0.68300781250000009</v>
+        <v>0.67812500000000009</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -911,7 +1020,45 @@
       </c>
       <c r="B23">
         <f>C20-B17</f>
-        <v>1.4837890625000001</v>
+        <v>1.4789062500000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26">
+        <f>ROUND(B25*1024/5000,0)</f>
+        <v>251</v>
+      </c>
+      <c r="C26">
+        <f>B26*5000/1024</f>
+        <v>1225.5859375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28">
+        <f>B25-B27</f>
+        <v>978</v>
       </c>
     </row>
   </sheetData>
@@ -919,11 +1066,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073D3162-803F-415C-B518-404A37595211}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1371,7 +1518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1490,7 +1637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824E6524-B061-4F2B-88F7-CA3E31CEFDE1}">
   <dimension ref="A1:J15"/>
   <sheetViews>

</xml_diff>

<commit_message>
can stuff implemented, sensor and heater handling corrected and improved, ....
</commit_message>
<xml_diff>
--- a/hardware/Datasheet/berechnungen.xlsx
+++ b/hardware/Datasheet/berechnungen.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D45516-964E-4F41-83A0-11D27DB1E505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5647A7-B5D2-4864-99B0-8332DDFDD835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PWM" sheetId="1" r:id="rId1"/>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +704,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>64</v>
+        <v>256</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -715,7 +715,7 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -723,8 +723,8 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <f>POWER(2,10)-1</f>
-        <v>1023</v>
+        <f>POWER(2,B3)-1</f>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -779,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED533D4-38E1-42C6-9DE3-B349AD92F31E}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>